<commit_message>
convert logic to import books by isbn
</commit_message>
<xml_diff>
--- a/src/main/resources/SampleExcelWorkbook.xlsx
+++ b/src/main/resources/SampleExcelWorkbook.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vineethvenudasan/code/hello-excel-boot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vineethvenudasan/vyvyd/excel-read-with-boot/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B2B79-736F-E34A-BD2E-3E2AC1C69B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D864370E-B855-B74A-95A5-E95F4D9B7089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{D12A4266-7CBE-6040-973B-4053FE8C2E15}"/>
   </bookViews>
   <sheets>
-    <sheet name="Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Import" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,31 +35,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Name</t>
+    <t>ISBN</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>978-1338216660</t>
   </si>
   <si>
-    <t>Max Maximillian</t>
-  </si>
-  <si>
-    <t>Maria Mustermann</t>
-  </si>
-  <si>
-    <t>maria.mustermann@email.com</t>
-  </si>
-  <si>
-    <t>max.maximillian@email.com</t>
+    <t>978-0590353427</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -73,14 +62,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,17 +84,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,47 +404,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE04E53-8D4C-7246-B5A7-5B9ABA338211}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B37A2A33-3A25-B641-8301-8C8617994591}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{0D74AB94-C547-2042-9667-1FFC829C3F7E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated test file (excel) with 5 rows of isbns
</commit_message>
<xml_diff>
--- a/src/main/resources/SampleExcelWorkbook.xlsx
+++ b/src/main/resources/SampleExcelWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vineethvenudasan/vyvyd/excel-read-with-boot/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D864370E-B855-B74A-95A5-E95F4D9B7089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8758F87C-54B0-3149-B7D8-C1AD23857D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{D12A4266-7CBE-6040-973B-4053FE8C2E15}"/>
   </bookViews>
@@ -35,15 +35,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ISBN</t>
   </si>
   <si>
-    <t>978-1338216660</t>
-  </si>
-  <si>
-    <t>978-0590353427</t>
+    <t>9780006479888</t>
+  </si>
+  <si>
+    <t>9781338216660</t>
+  </si>
+  <si>
+    <t>9780590353427</t>
+  </si>
+  <si>
+    <t>9780141199702</t>
+  </si>
+  <si>
+    <t>9780201835953</t>
   </si>
 </sst>
 </file>
@@ -87,9 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE04E53-8D4C-7246-B5A7-5B9ABA338211}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -421,13 +431,28 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>